<commit_message>
updated IO files from consultant
</commit_message>
<xml_diff>
--- a/InputData/io-model/BGDP/BAU GDP.xlsx
+++ b/InputData/io-model/BGDP/BAU GDP.xlsx
@@ -1,25 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\add-outputs\BGDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarrynna\Dropbox (CEA)\Energy Innovation IO\Deliverable IO files\Canada\BGDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C5FFC3-857E-4CD0-8096-9781F5BAB6F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23415" windowHeight="11310"/>
+    <workbookView xWindow="33840" yWindow="2175" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="OECD Data" sheetId="3" r:id="rId2"/>
     <sheet name="BGDP" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -70,12 +80,6 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>GDPLTFORECAST</t>
   </si>
   <si>
@@ -104,12 +108,18 @@
   </si>
   <si>
     <t>Unit: 2012 USD</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>CAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,7 +184,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -182,6 +191,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -462,10 +472,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -517,12 +529,12 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -530,7 +542,7 @@
         <v>1.0529130131709286</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -539,12 +551,12 @@
         <v>1000000</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -552,10 +564,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -587,1088 +601,1088 @@
         <v>13</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <v>2014</v>
       </c>
-      <c r="G2">
-        <v>16208167.451801199</v>
+      <c r="G2" s="8">
+        <v>1505495.47140106</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>2015</v>
       </c>
-      <c r="G3" s="5">
-        <v>16671978.001079099</v>
+      <c r="G3" s="8">
+        <v>1520564.3540934401</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>2016</v>
       </c>
-      <c r="G4">
-        <v>16919603.417713501</v>
+      <c r="G4" s="8">
+        <v>1542066.2592517899</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>2017</v>
       </c>
-      <c r="G5">
-        <v>17304243.025623702</v>
+      <c r="G5" s="8">
+        <v>1588338.69301313</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <v>2018</v>
       </c>
-      <c r="G6">
-        <v>17798638.6604435</v>
+      <c r="G6" s="8">
+        <v>1621635.5389815201</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7">
         <v>2019</v>
       </c>
-      <c r="G7">
-        <v>18292645.569375802</v>
+      <c r="G7" s="8">
+        <v>1657928.8942838099</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8">
         <v>2020</v>
       </c>
-      <c r="G8">
-        <v>18587190</v>
+      <c r="G8" s="8">
+        <v>1684775</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9">
         <v>2021</v>
       </c>
-      <c r="G9">
-        <v>18849540</v>
+      <c r="G9" s="8">
+        <v>1710503</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10">
         <v>2022</v>
       </c>
-      <c r="G10">
-        <v>19124900</v>
+      <c r="G10" s="8">
+        <v>1736864</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11">
         <v>2023</v>
       </c>
-      <c r="G11">
-        <v>19422190</v>
+      <c r="G11" s="8">
+        <v>1764255</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12">
         <v>2024</v>
       </c>
-      <c r="G12">
-        <v>19740540</v>
+      <c r="G12" s="8">
+        <v>1792774</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13">
         <v>2025</v>
       </c>
-      <c r="G13">
-        <v>20075600</v>
+      <c r="G13" s="8">
+        <v>1822387</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F14">
         <v>2026</v>
       </c>
-      <c r="G14">
-        <v>20424180</v>
+      <c r="G14" s="8">
+        <v>1852965</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F15">
         <v>2027</v>
       </c>
-      <c r="G15">
-        <v>20784020</v>
+      <c r="G15" s="8">
+        <v>1884677</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F16">
         <v>2028</v>
       </c>
-      <c r="G16">
-        <v>21153450</v>
+      <c r="G16" s="8">
+        <v>1917532</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F17">
         <v>2029</v>
       </c>
-      <c r="G17">
-        <v>21531180</v>
+      <c r="G17" s="8">
+        <v>1951559</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F18">
         <v>2030</v>
       </c>
-      <c r="G18">
-        <v>21916430</v>
+      <c r="G18" s="8">
+        <v>1986793</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F19">
         <v>2031</v>
       </c>
-      <c r="G19">
-        <v>22309050</v>
+      <c r="G19" s="8">
+        <v>2023273</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F20">
         <v>2032</v>
       </c>
-      <c r="G20">
-        <v>22709530</v>
+      <c r="G20" s="8">
+        <v>2060808</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F21">
         <v>2033</v>
       </c>
-      <c r="G21">
-        <v>23118740</v>
+      <c r="G21" s="8">
+        <v>2099401</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F22">
         <v>2034</v>
       </c>
-      <c r="G22">
-        <v>23537610</v>
+      <c r="G22" s="8">
+        <v>2139034</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F23">
         <v>2035</v>
       </c>
-      <c r="G23">
-        <v>23967030</v>
+      <c r="G23" s="8">
+        <v>2179688</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F24">
         <v>2036</v>
       </c>
-      <c r="G24">
-        <v>24407860</v>
+      <c r="G24" s="8">
+        <v>2221353</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F25">
         <v>2037</v>
       </c>
-      <c r="G25">
-        <v>24861010</v>
+      <c r="G25" s="8">
+        <v>2264030</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F26">
         <v>2038</v>
       </c>
-      <c r="G26">
-        <v>25327180</v>
+      <c r="G26" s="8">
+        <v>2307720</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F27">
         <v>2039</v>
       </c>
-      <c r="G27">
-        <v>25806800</v>
+      <c r="G27" s="8">
+        <v>2352425</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F28">
         <v>2040</v>
       </c>
-      <c r="G28">
-        <v>26300140</v>
+      <c r="G28" s="8">
+        <v>2398151</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F29">
         <v>2041</v>
       </c>
-      <c r="G29">
-        <v>26807420</v>
+      <c r="G29" s="8">
+        <v>2444905</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F30">
         <v>2042</v>
       </c>
-      <c r="G30">
-        <v>27328940</v>
+      <c r="G30" s="8">
+        <v>2492690</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F31">
         <v>2043</v>
       </c>
-      <c r="G31">
-        <v>27864750</v>
+      <c r="G31" s="8">
+        <v>2541479</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F32">
         <v>2044</v>
       </c>
-      <c r="G32">
-        <v>28414590</v>
+      <c r="G32" s="8">
+        <v>2591227</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F33">
         <v>2045</v>
       </c>
-      <c r="G33">
-        <v>28978050</v>
+      <c r="G33" s="8">
+        <v>2641896</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F34">
         <v>2046</v>
       </c>
-      <c r="G34">
-        <v>29554850</v>
+      <c r="G34" s="8">
+        <v>2693479</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F35">
         <v>2047</v>
       </c>
-      <c r="G35">
-        <v>30144870</v>
+      <c r="G35" s="8">
+        <v>2745988</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F36">
         <v>2048</v>
       </c>
-      <c r="G36">
-        <v>30747840</v>
+      <c r="G36" s="8">
+        <v>2799434</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F37">
         <v>2049</v>
       </c>
-      <c r="G37">
-        <v>31363330</v>
+      <c r="G37" s="8">
+        <v>2853831</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F38">
         <v>2050</v>
       </c>
-      <c r="G38">
-        <v>31990910</v>
+      <c r="G38" s="8">
+        <v>2909216</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F39">
         <v>2051</v>
       </c>
-      <c r="G39">
-        <v>32630430</v>
+      <c r="G39" s="8">
+        <v>2965657</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F40">
         <v>2052</v>
       </c>
-      <c r="G40">
-        <v>33282110</v>
+      <c r="G40" s="8">
+        <v>3023227</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F41">
         <v>2053</v>
       </c>
-      <c r="G41">
-        <v>33946130</v>
+      <c r="G41" s="8">
+        <v>3081985</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E42" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F42">
         <v>2054</v>
       </c>
-      <c r="G42">
-        <v>34622620</v>
+      <c r="G42" s="8">
+        <v>3141981</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F43">
         <v>2055</v>
       </c>
-      <c r="G43">
-        <v>35311770</v>
+      <c r="G43" s="8">
+        <v>3203277</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F44">
         <v>2056</v>
       </c>
-      <c r="G44">
-        <v>36014100</v>
+      <c r="G44" s="8">
+        <v>3265966</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F45">
         <v>2057</v>
       </c>
-      <c r="G45">
-        <v>36730540</v>
+      <c r="G45" s="8">
+        <v>3330145</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E46" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F46">
         <v>2058</v>
       </c>
-      <c r="G46">
-        <v>37462060</v>
+      <c r="G46" s="8">
+        <v>3395881</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E47" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F47">
         <v>2059</v>
       </c>
-      <c r="G47">
-        <v>38209630</v>
+      <c r="G47" s="8">
+        <v>3463205</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F48">
         <v>2060</v>
       </c>
-      <c r="G48">
-        <v>38974320</v>
+      <c r="G48" s="8">
+        <v>3532133</v>
       </c>
     </row>
   </sheetData>
@@ -1677,449 +1691,451 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>20</v>
+      <c r="A1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2014</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <f>'OECD Data'!G2*About!$A$15*About!$A$16</f>
-        <v>17065790429654.971</v>
+        <v>1585155773108.0776</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2015</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <f>'OECD Data'!G3*About!$A$15*About!$A$16</f>
-        <v>17554142592635.627</v>
+        <v>1601021995788.8308</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2016</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <f>'OECD Data'!G4*About!$A$15*About!$A$16</f>
-        <v>17814870616201.863</v>
+        <v>1623661631538.0244</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2017</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <f>'OECD Data'!G5*About!$A$15*About!$A$16</f>
-        <v>18219862664751.477</v>
+        <v>1672382479196.4292</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2018</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <f>'OECD Data'!G6*About!$A$15*About!$A$16</f>
-        <v>18740418262308.145</v>
+        <v>1707441161614.0952</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2019</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <f>'OECD Data'!G7*About!$A$15*About!$A$16</f>
-        <v>19260564565319.313</v>
+        <v>1745654907703.5122</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2020</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <f>'OECD Data'!G8*About!$A$15*About!$A$16</f>
-        <v>19570694229280.551</v>
+        <v>1773921521765.0513</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2021</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <f>'OECD Data'!G9*About!$A$15*About!$A$16</f>
-        <v>19846925958285.945</v>
+        <v>1801010867767.9128</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2022</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <f>'OECD Data'!G10*About!$A$15*About!$A$16</f>
-        <v>20136856085592.691</v>
+        <v>1828766707708.1118</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2023</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <f>'OECD Data'!G11*About!$A$15*About!$A$16</f>
-        <v>20449876595278.277</v>
+        <v>1857607048051.8765</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2024</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <f>'OECD Data'!G12*About!$A$15*About!$A$16</f>
-        <v>20785071453021.242</v>
+        <v>1887635074274.4983</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2025</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <f>'OECD Data'!G13*About!$A$15*About!$A$16</f>
-        <v>21137860487214.293</v>
+        <v>1918814987333.5288</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2026</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <f>'OECD Data'!G14*About!$A$15*About!$A$16</f>
-        <v>21504884905345.414</v>
+        <v>1951010961450.2698</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2027</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <f>'OECD Data'!G15*About!$A$15*About!$A$16</f>
-        <v>21883765124004.84</v>
+        <v>1984400938923.946</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2028</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <f>'OECD Data'!G16*About!$A$15*About!$A$16</f>
-        <v>22272742778460.578</v>
+        <v>2018994395971.677</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2029</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <f>'OECD Data'!G17*About!$A$15*About!$A$16</f>
-        <v>22670459610925.633</v>
+        <v>2054821867070.8442</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2030</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <f>'OECD Data'!G18*About!$A$15*About!$A$16</f>
-        <v>23076094349249.734</v>
+        <v>2091920204176.9087</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2031</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <f>'OECD Data'!G19*About!$A$15*About!$A$16</f>
-        <v>23489489056480.902</v>
+        <v>2130330470897.384</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2032</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <f>'OECD Data'!G20*About!$A$15*About!$A$16</f>
-        <v>23911159659995.598</v>
+        <v>2169851560846.7549</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2033</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <f>'OECD Data'!G21*About!$A$15*About!$A$16</f>
-        <v>24342022194115.273</v>
+        <v>2210486632764.0605</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2034</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <f>'OECD Data'!G22*About!$A$15*About!$A$16</f>
-        <v>24783055867942.18</v>
+        <v>2252216734215.064</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2035</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <f>'OECD Data'!G23*About!$A$15*About!$A$16</f>
-        <v>25235197774058.039</v>
+        <v>2295021859852.5146</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2036</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <f>'OECD Data'!G24*About!$A$15*About!$A$16</f>
-        <v>25699353417654.18</v>
+        <v>2338891480546.2817</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2037</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <f>'OECD Data'!G25*About!$A$15*About!$A$16</f>
-        <v>26176480949572.586</v>
+        <v>2383826649209.3774</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2038</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <f>'OECD Data'!G26*About!$A$15*About!$A$16</f>
-        <v>26667317408922.48</v>
+        <v>2429828418754.8149</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2039</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <f>'OECD Data'!G27*About!$A$15*About!$A$16</f>
-        <v>27172315548299.516</v>
+        <v>2476898895008.6216</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2040</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <f>'OECD Data'!G28*About!$A$15*About!$A$16</f>
-        <v>27691759654217.266</v>
+        <v>2525044395448.8755</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2041</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <f>'OECD Data'!G29*About!$A$15*About!$A$16</f>
-        <v>28225881367538.613</v>
+        <v>2574272290466.6689</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2042</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <f>'OECD Data'!G30*About!$A$15*About!$A$16</f>
-        <v>28774996562167.52</v>
+        <v>2624585738801.042</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2043</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <f>'OECD Data'!G31*About!$A$15*About!$A$16</f>
-        <v>29339157883754.633</v>
+        <v>2675956311800.6382</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2044</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <f>'OECD Data'!G32*About!$A$15*About!$A$16</f>
-        <v>29918091574916.535</v>
+        <v>2728336628379.8657</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2045</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <f>'OECD Data'!G33*About!$A$15*About!$A$16</f>
-        <v>30511365941317.828</v>
+        <v>2781686677844.2236</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2046</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <f>'OECD Data'!G34*About!$A$15*About!$A$16</f>
-        <v>31118686167314.816</v>
+        <v>2835999089802.6196</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2047</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <f>'OECD Data'!G35*About!$A$15*About!$A$16</f>
-        <v>31739925903345.926</v>
+        <v>2891286499211.2119</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2048</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <f>'OECD Data'!G36*About!$A$15*About!$A$16</f>
-        <v>32374800862897.605</v>
+        <v>2947560488113.1455</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2049</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <f>'OECD Data'!G37*About!$A$15*About!$A$16</f>
-        <v>33022858293374.176</v>
+        <v>3004835797290.604</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2050</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="6">
         <f>'OECD Data'!G38*About!$A$15*About!$A$16</f>
-        <v>33683645442179.992</v>
+        <v>3063151384525.0762</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2051</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="6">
         <f>'OECD Data'!G39*About!$A$15*About!$A$16</f>
-        <v>34357004372363.063</v>
+        <v>3122578847901.4565</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2052</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="6">
         <f>'OECD Data'!G40*About!$A$15*About!$A$16</f>
-        <v>35043166724786.297</v>
+        <v>3183195050069.707</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2053</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="6">
         <f>'OECD Data'!G41*About!$A$15*About!$A$16</f>
-        <v>35742322023792.047</v>
+        <v>3245062112897.604</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2054</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="6">
         <f>'OECD Data'!G42*About!$A$15*About!$A$16</f>
-        <v>36454607148072.055</v>
+        <v>3308232682035.8071</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2055</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="6">
         <f>'OECD Data'!G43*About!$A$15*About!$A$16</f>
-        <v>37180222151098.805</v>
+        <v>3372772038091.1323</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2056</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="6">
         <f>'OECD Data'!G44*About!$A$15*About!$A$16</f>
-        <v>37919714547639.141</v>
+        <v>3438778101973.8047</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2057</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="6">
         <f>'OECD Data'!G45*About!$A$15*About!$A$16</f>
-        <v>38674063546795.313</v>
+        <v>3506353006246.1021</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2058</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="6">
         <f>'OECD Data'!G46*About!$A$15*About!$A$16</f>
-        <v>39444290474190.117</v>
+        <v>3575567296079.9063</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2059</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="6">
         <f>'OECD Data'!G47*About!$A$15*About!$A$16</f>
-        <v>40231416655446.305</v>
+        <v>3646453611778.626</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2060</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="6">
         <f>'OECD Data'!G48*About!$A$15*About!$A$16</f>
-        <v>41036568707487.984</v>
+        <v>3719028799950.4717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>